<commit_message>
Changes Done for Test Data applied in the main class
</commit_message>
<xml_diff>
--- a/KeywordDriven_Framework/ExcelTestFiles/TestScript.xlsx
+++ b/KeywordDriven_Framework/ExcelTestFiles/TestScript.xlsx
@@ -16,6 +16,7 @@
     <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>S..No</t>
   </si>
@@ -126,7 +127,7 @@
     <t>Iterate</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -192,7 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -207,7 +208,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -502,7 +502,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +518,7 @@
       <c r="A1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -548,7 +548,7 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -561,7 +561,7 @@
       <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -572,7 +572,7 @@
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -589,7 +589,7 @@
       <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -606,7 +606,7 @@
       <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -623,7 +623,7 @@
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -638,7 +638,7 @@
       <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -655,7 +655,7 @@
       <c r="D10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -672,7 +672,7 @@
       <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -683,7 +683,7 @@
       <c r="D12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -694,7 +694,7 @@
       <c r="D13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -705,7 +705,7 @@
       <c r="D14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -716,7 +716,7 @@
       <c r="D15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -726,11 +726,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -740,7 +738,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -761,13 +759,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>